<commit_message>
Fixed the File Merge Issue
</commit_message>
<xml_diff>
--- a/Audio_Files/Person_1/Comparison_Sentences/SIT.xlsx
+++ b/Audio_Files/Person_1/Comparison_Sentences/SIT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cvkrishnarao/Desktop/RA/Intelligibility_Software_Module/Audio_Files/Person_1/Comparison_Sentences/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382133CF-10E6-8E4C-A3A8-AD2AF7E4D527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CC08F2-11B8-C349-90AA-86578528C50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="29920" windowHeight="18680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,55 +20,67 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>P1_W1_S2</t>
   </si>
   <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>P1_W1_S5</t>
-  </si>
-  <si>
     <t>P1_W1_S1</t>
   </si>
   <si>
-    <t>Test4</t>
-  </si>
-  <si>
     <t>P1_W1_S4</t>
   </si>
   <si>
-    <t>Test5</t>
-  </si>
-  <si>
-    <t>P1_W1_S6</t>
-  </si>
-  <si>
-    <t>Test6</t>
-  </si>
-  <si>
     <t>P1_W1_S3</t>
   </si>
   <si>
     <t>NAME</t>
   </si>
   <si>
-    <t>Test1123</t>
-  </si>
-  <si>
-    <t>Test3234</t>
-  </si>
-  <si>
     <t>SENTENCES</t>
+  </si>
+  <si>
+    <t>We picked grapes for wine</t>
+  </si>
+  <si>
+    <t>The ballet is about to begin.</t>
+  </si>
+  <si>
+    <t>You're used to being on the field.</t>
+  </si>
+  <si>
+    <t>Enjoy the fair weather while in the tropics.</t>
+  </si>
+  <si>
+    <t>I think I'm getting better.</t>
+  </si>
+  <si>
+    <t>P1_W2_S1</t>
+  </si>
+  <si>
+    <t>You want him to do well</t>
+  </si>
+  <si>
+    <t>P1_W2_S2</t>
+  </si>
+  <si>
+    <t>Big muscles are not necessarily strong ones</t>
+  </si>
+  <si>
+    <t>P1_W2_S3</t>
+  </si>
+  <si>
+    <t>he is capable and willing to make decisions.</t>
+  </si>
+  <si>
+    <t>P1_W2_S4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +92,18 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -117,11 +141,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,70 +450,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>11</v>
+      <c r="A2" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>12</v>
+      <c r="A4" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
+      <c r="A5" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>